<commit_message>
Actualizacion fotos y figuras
</commit_message>
<xml_diff>
--- a/experimento regeneracion/Datos experimento regen.xlsx
+++ b/experimento regeneracion/Datos experimento regen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\collf\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\collf\Documents\GitHub\Revision_datos_TFG\experimento regeneracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E577018-5B8F-45DF-A7F8-08952F01CBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58867C6C-C3AF-4039-975A-378984447A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{03B35580-133D-4DB9-8E55-46A9E8197AA7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
   <si>
     <t>n</t>
   </si>
@@ -33,9 +33,6 @@
     <t>tiempo</t>
   </si>
   <si>
-    <t>T7</t>
-  </si>
-  <si>
     <t>peso (g)</t>
   </si>
   <si>
@@ -46,12 +43,27 @@
   </si>
   <si>
     <t>fecha de corte</t>
+  </si>
+  <si>
+    <t>t7d</t>
+  </si>
+  <si>
+    <t>t24h</t>
+  </si>
+  <si>
+    <t>t0h</t>
+  </si>
+  <si>
+    <t>t6h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,9 +93,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -102,7 +116,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -398,13 +412,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECDA251-8395-46AE-A8F0-D7F799EC57D9}">
-  <dimension ref="A2:E6"/>
+  <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -414,16 +428,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -434,10 +448,10 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1">
         <v>45912</v>
@@ -451,10 +465,10 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1">
         <v>45912</v>
@@ -468,10 +482,10 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1">
         <v>45912</v>
@@ -485,13 +499,178 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
         <v>45912</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>45919</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="3">
+        <f>AVERAGE(B3:B15)</f>
+        <v>33.230769230769234</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="2">
+        <f>_xlfn.STDEV.S(B3:B15)</f>
+        <v>16.588921233531359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>